<commit_message>
FIX: Remove redundant Cells in solvency2
</commit_message>
<xml_diff>
--- a/lifelib/projects/solvency2/model/Input/input.xlsx
+++ b/lifelib/projects/solvency2/model/Input/input.xlsx
@@ -660,7 +660,7 @@
       <selection activeCell="B7" sqref="B7:O307"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col width="20.7265625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.36328125" customWidth="1" style="1" min="2" max="2"/>
@@ -14772,7 +14772,7 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.08984375" defaultRowHeight="12.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
     <col width="6.7265625" customWidth="1" style="4" min="1" max="1"/>
     <col width="9.6328125" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
@@ -19621,7 +19621,7 @@
       <selection activeCell="B7" sqref="B7:V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col width="11.36328125" customWidth="1" style="1" min="1" max="1"/>
     <col width="10.36328125" customWidth="1" style="1" min="2" max="2"/>
@@ -20324,7 +20324,7 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.5"/>
   <cols>
     <col width="5.6328125" customWidth="1" style="18" min="1" max="1"/>
     <col width="5" bestFit="1" customWidth="1" style="18" min="2" max="2"/>
@@ -20441,7 +20441,7 @@
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col width="10.7265625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="11.7265625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -20927,7 +20927,7 @@
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col width="9" customWidth="1" style="1" min="1" max="1"/>
     <col width="8" customWidth="1" style="1" min="2" max="2"/>
@@ -21607,7 +21607,7 @@
       <selection activeCell="F1477" sqref="F1477"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col width="7.7265625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="8.1796875" customWidth="1" style="1" min="2" max="2"/>

</xml_diff>

<commit_message>
CHG: Update solvency2 to address modelx change
</commit_message>
<xml_diff>
--- a/lifelib/projects/solvency2/model/Input/input.xlsx
+++ b/lifelib/projects/solvency2/model/Input/input.xlsx
@@ -360,6 +360,74 @@
     <cellStyle name="パーセント" xfId="2" builtinId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 

</xml_diff>

<commit_message>
CHG: Remove model scripts from projects
</commit_message>
<xml_diff>
--- a/lifelib/projects/solvency2/model/Input/input.xlsx
+++ b/lifelib/projects/solvency2/model/Input/input.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="80" yWindow="80" windowWidth="24930" windowHeight="12940" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolicyData" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mortality" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProductSpec" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OtherParams" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assumption" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssumptionTables" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scenarios" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="PolicyData" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Mortality" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ProductSpec" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="OtherParams" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Assumption" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="AssumptionTables" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Scenarios" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="AsmpByDuration">AssumptionTables!$B$7:$J$27</definedName>
@@ -19665,12 +19665,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="P5:Q5"/>
     <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" scale="98"/>

</xml_diff>